<commit_message>
made smf work the same way as sinclair
</commit_message>
<xml_diff>
--- a/owlcms/src/main/resources/agegroups/AgeGroups.xlsx
+++ b/owlcms/src/main/resources/agegroups/AgeGroups.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\owlcms4\owlcms\src\main\resources\agegroups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D03797C7-69FE-42BD-8339-DAD31697C5F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3FF8447-B5FD-4E43-8BF5-7609410E0349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BW Categories" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="72">
   <si>
     <t>code</t>
   </si>
@@ -207,9 +207,6 @@
   </si>
   <si>
     <t>JR</t>
-  </si>
-  <si>
-    <t>ALL</t>
   </si>
   <si>
     <t>DEFAULT</t>
@@ -1079,8 +1076,8 @@
   </sheetPr>
   <dimension ref="A1:U44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1987,7 +1984,7 @@
     </row>
     <row r="18" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="1" t="s">
@@ -2262,11 +2259,11 @@
     </row>
     <row r="23" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>30</v>
@@ -2629,7 +2626,7 @@
     </row>
     <row r="30" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B30" s="5"/>
       <c r="C30" s="1" t="s">
@@ -2849,7 +2846,7 @@
     </row>
     <row r="34" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="1" t="s">
@@ -2959,7 +2956,7 @@
     </row>
     <row r="36" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B36" s="5"/>
       <c r="C36" s="1" t="s">
@@ -3014,7 +3011,7 @@
     </row>
     <row r="37" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B37" s="5"/>
       <c r="C37" s="1" t="s">
@@ -3069,7 +3066,7 @@
     </row>
     <row r="38" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="1" t="s">
@@ -3124,7 +3121,7 @@
     </row>
     <row r="39" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B39" s="5"/>
       <c r="C39" s="1" t="s">
@@ -3179,7 +3176,7 @@
     </row>
     <row r="40" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B40" s="5"/>
       <c r="C40" s="1" t="s">
@@ -3399,11 +3396,11 @@
     </row>
     <row r="44" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
new masters age groups
</commit_message>
<xml_diff>
--- a/owlcms/src/main/resources/agegroups/AgeGroups.xlsx
+++ b/owlcms/src/main/resources/agegroups/AgeGroups.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\owlcms4\owlcms\src\main\resources\agegroups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3FF8447-B5FD-4E43-8BF5-7609410E0349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B337781E-6EDD-45E8-A710-E22AFECC5079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BW Categories" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="77">
   <si>
     <t>code</t>
   </si>
@@ -173,33 +173,12 @@
     <t>SR</t>
   </si>
   <si>
-    <t>F30</t>
-  </si>
-  <si>
     <t>MASTERS</t>
   </si>
   <si>
-    <t>F50</t>
-  </si>
-  <si>
-    <t>F60</t>
-  </si>
-  <si>
-    <t>F65</t>
-  </si>
-  <si>
-    <t>F70</t>
-  </si>
-  <si>
-    <t>F75</t>
-  </si>
-  <si>
     <t>F999 is always used as the last category in an age group</t>
   </si>
   <si>
-    <t>F70+</t>
-  </si>
-  <si>
     <t>YTH</t>
   </si>
   <si>
@@ -230,20 +209,56 @@
     <t>M75</t>
   </si>
   <si>
-    <t>M80+</t>
-  </si>
-  <si>
-    <t>F80+</t>
-  </si>
-  <si>
     <t>Open</t>
+  </si>
+  <si>
+    <t>W30</t>
+  </si>
+  <si>
+    <t>W35</t>
+  </si>
+  <si>
+    <t>W40</t>
+  </si>
+  <si>
+    <t>W45</t>
+  </si>
+  <si>
+    <t>W50</t>
+  </si>
+  <si>
+    <t>W55</t>
+  </si>
+  <si>
+    <t>W60</t>
+  </si>
+  <si>
+    <t>W65</t>
+  </si>
+  <si>
+    <t>W70</t>
+  </si>
+  <si>
+    <t>W75</t>
+  </si>
+  <si>
+    <t>W80</t>
+  </si>
+  <si>
+    <t>W85</t>
+  </si>
+  <si>
+    <t>M80</t>
+  </si>
+  <si>
+    <t>M85</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -277,6 +292,22 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -304,7 +335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -318,8 +349,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1057,7 +1098,7 @@
         <v>255</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1074,10 +1115,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:U44"/>
+  <dimension ref="A1:U45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G38" sqref="G37:G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1105,11 +1146,11 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
       <c r="K1" s="7"/>
       <c r="L1" s="7"/>
       <c r="M1" s="7"/>
@@ -1434,11 +1475,11 @@
     </row>
     <row r="8" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>30</v>
@@ -1489,11 +1530,11 @@
     </row>
     <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>30</v>
@@ -1544,11 +1585,11 @@
     </row>
     <row r="10" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>30</v>
@@ -1599,11 +1640,11 @@
     </row>
     <row r="11" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>30</v>
@@ -1654,11 +1695,11 @@
     </row>
     <row r="12" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>30</v>
@@ -1709,11 +1750,11 @@
     </row>
     <row r="13" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>30</v>
@@ -1764,11 +1805,11 @@
     </row>
     <row r="14" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>30</v>
@@ -1819,11 +1860,11 @@
     </row>
     <row r="15" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>30</v>
@@ -1874,11 +1915,11 @@
     </row>
     <row r="16" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>30</v>
@@ -1929,11 +1970,11 @@
     </row>
     <row r="17" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>30</v>
@@ -1984,11 +2025,11 @@
     </row>
     <row r="18" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>30</v>
@@ -1997,7 +2038,7 @@
         <v>80</v>
       </c>
       <c r="F18" s="4">
-        <v>999</v>
+        <v>84</v>
       </c>
       <c r="G18" s="8" t="b">
         <v>0</v>
@@ -2037,68 +2078,68 @@
       <c r="T18" s="5"/>
       <c r="U18" s="5"/>
     </row>
-    <row r="19" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D19" s="1" t="s">
+    <row r="19" spans="1:21" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="4">
-        <v>70</v>
-      </c>
-      <c r="F19" s="4">
+      <c r="E19" s="14">
+        <v>85</v>
+      </c>
+      <c r="F19" s="14">
         <v>999</v>
       </c>
-      <c r="G19" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="H19" s="5"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1" t="s">
+      <c r="G19" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="K19" s="1" t="s">
+      <c r="K19" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="L19" s="1" t="s">
+      <c r="L19" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="M19" s="1" t="s">
+      <c r="M19" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="N19" s="1" t="s">
+      <c r="N19" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="O19" s="1" t="s">
+      <c r="O19" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="P19" s="1" t="s">
+      <c r="P19" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="Q19" s="1" t="s">
+      <c r="Q19" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="R19" s="1" t="s">
+      <c r="R19" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="S19" s="1" t="s">
+      <c r="S19" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="T19" s="5"/>
-      <c r="U19" s="5"/>
+      <c r="T19" s="13"/>
+      <c r="U19" s="13"/>
     </row>
     <row r="20" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>30</v>
@@ -2149,11 +2190,11 @@
     </row>
     <row r="21" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>30</v>
@@ -2208,7 +2249,7 @@
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>30</v>
@@ -2259,11 +2300,11 @@
     </row>
     <row r="23" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>30</v>
@@ -2626,11 +2667,11 @@
     </row>
     <row r="30" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B30" s="5"/>
       <c r="C30" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>12</v>
@@ -2685,7 +2726,7 @@
       </c>
       <c r="B31" s="5"/>
       <c r="C31" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>12</v>
@@ -2740,7 +2781,7 @@
       </c>
       <c r="B32" s="5"/>
       <c r="C32" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>12</v>
@@ -2795,7 +2836,7 @@
       </c>
       <c r="B33" s="5"/>
       <c r="C33" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>12</v>
@@ -2846,11 +2887,11 @@
     </row>
     <row r="34" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>12</v>
@@ -2905,7 +2946,7 @@
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>12</v>
@@ -2956,11 +2997,11 @@
     </row>
     <row r="36" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B36" s="5"/>
       <c r="C36" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>12</v>
@@ -3011,11 +3052,11 @@
     </row>
     <row r="37" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B37" s="5"/>
       <c r="C37" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>12</v>
@@ -3066,11 +3107,11 @@
     </row>
     <row r="38" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>12</v>
@@ -3121,11 +3162,11 @@
     </row>
     <row r="39" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B39" s="5"/>
       <c r="C39" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>12</v>
@@ -3174,22 +3215,22 @@
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>69</v>
+    <row r="40" spans="1:21" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A40" s="12" t="s">
+        <v>75</v>
       </c>
       <c r="B40" s="5"/>
-      <c r="C40" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D40" s="1" t="s">
+      <c r="C40" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D40" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E40" s="4">
         <v>80</v>
       </c>
       <c r="F40" s="4">
-        <v>999</v>
+        <v>84</v>
       </c>
       <c r="G40" s="8" t="b">
         <v>0</v>
@@ -3198,53 +3239,53 @@
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
       <c r="K40" s="5"/>
-      <c r="L40" s="1" t="s">
+      <c r="L40" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="M40" s="1" t="s">
+      <c r="M40" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="N40" s="1" t="s">
+      <c r="N40" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="O40" s="1" t="s">
+      <c r="O40" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="P40" s="1" t="s">
+      <c r="P40" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="Q40" s="1" t="s">
+      <c r="Q40" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="R40" s="1" t="s">
+      <c r="R40" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="S40" s="1" t="s">
+      <c r="S40" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="T40" s="1" t="s">
+      <c r="T40" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="U40" s="1" t="s">
+      <c r="U40" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="41" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>59</v>
+      <c r="A41" s="12" t="s">
+        <v>76</v>
       </c>
       <c r="B41" s="5"/>
       <c r="C41" s="1" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E41" s="4">
-        <v>13</v>
+        <v>85</v>
       </c>
       <c r="F41" s="4">
-        <v>17</v>
+        <v>999</v>
       </c>
       <c r="G41" s="8" t="b">
         <v>0</v>
@@ -3252,9 +3293,7 @@
       <c r="H41" s="5"/>
       <c r="I41" s="5"/>
       <c r="J41" s="5"/>
-      <c r="K41" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="K41" s="5"/>
       <c r="L41" s="1" t="s">
         <v>18</v>
       </c>
@@ -3280,26 +3319,28 @@
         <v>25</v>
       </c>
       <c r="T41" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U41" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="U41" s="5"/>
     </row>
     <row r="42" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B42" s="5"/>
       <c r="C42" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E42" s="4">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F42" s="4">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G42" s="8" t="b">
         <v>0</v>
@@ -3307,7 +3348,9 @@
       <c r="H42" s="5"/>
       <c r="I42" s="5"/>
       <c r="J42" s="5"/>
-      <c r="K42" s="5"/>
+      <c r="K42" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="L42" s="1" t="s">
         <v>18</v>
       </c>
@@ -3333,19 +3376,17 @@
         <v>25</v>
       </c>
       <c r="T42" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="U42" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="U42" s="5"/>
     </row>
     <row r="43" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B43" s="5"/>
       <c r="C43" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>12</v>
@@ -3354,7 +3395,7 @@
         <v>15</v>
       </c>
       <c r="F43" s="4">
-        <v>999</v>
+        <v>20</v>
       </c>
       <c r="G43" s="8" t="b">
         <v>0</v>
@@ -3396,36 +3437,28 @@
     </row>
     <row r="44" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E44" s="4">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F44" s="4">
         <v>999</v>
       </c>
       <c r="G44" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I44" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J44" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K44" s="1" t="s">
-        <v>17</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
+      <c r="J44" s="5"/>
+      <c r="K44" s="5"/>
       <c r="L44" s="1" t="s">
         <v>18</v>
       </c>
@@ -3454,6 +3487,69 @@
         <v>26</v>
       </c>
       <c r="U44" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B45" s="5"/>
+      <c r="C45" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E45" s="4">
+        <v>0</v>
+      </c>
+      <c r="F45" s="4">
+        <v>999</v>
+      </c>
+      <c r="G45" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M45" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N45" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O45" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P45" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q45" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R45" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S45" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="T45" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U45" s="1" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3462,5 +3558,6 @@
     <mergeCell ref="H1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated AgeGroups with recent world records
</commit_message>
<xml_diff>
--- a/owlcms/src/main/resources/agegroups/AgeGroups.xlsx
+++ b/owlcms/src/main/resources/agegroups/AgeGroups.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\owlcms4\owlcms\src\main\resources\agegroups\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jefer\Downloads\Jeferson\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB3F12E-4BE5-44B6-A466-4AE3C024D34A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E25A078-35F3-4A04-8799-4ACA4E6E3CC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BW Categories" sheetId="1" r:id="rId1"/>
@@ -258,7 +258,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -308,8 +308,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -320,6 +326,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF8EA9DB"/>
         <bgColor rgb="FF8EA9DB"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -335,7 +347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -357,13 +369,20 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -585,293 +604,297 @@
   </sheetPr>
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="18">
         <v>35</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
       <c r="H2" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="18">
         <v>40</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8">
+        <v>135</v>
+      </c>
       <c r="H3" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="18">
         <v>45</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8">
+        <v>172</v>
+      </c>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="18">
         <v>49</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="15">
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="19">
         <v>221</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="18">
         <v>55</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="13">
         <v>294</v>
       </c>
-      <c r="E6" s="15">
-        <v>264</v>
-      </c>
-      <c r="F6" s="15">
-        <v>248</v>
+      <c r="E6" s="13">
+        <v>265</v>
+      </c>
+      <c r="F6" s="19">
+        <v>258</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="18">
         <v>61</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="13">
         <v>318</v>
       </c>
-      <c r="E7" s="15">
-        <v>293</v>
-      </c>
-      <c r="F7" s="16">
+      <c r="E7" s="13">
+        <v>307</v>
+      </c>
+      <c r="F7" s="14">
         <v>276</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="18">
         <v>67</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="13">
         <v>339</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="13">
         <v>328</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="13">
         <v>306</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="18">
         <v>73</v>
       </c>
-      <c r="D9" s="15">
-        <v>363</v>
-      </c>
-      <c r="E9" s="16">
-        <v>349</v>
-      </c>
-      <c r="F9" s="15">
-        <v>307</v>
+      <c r="D9" s="13">
+        <v>364</v>
+      </c>
+      <c r="E9" s="14">
+        <v>351</v>
+      </c>
+      <c r="F9" s="13">
+        <v>309</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="18">
         <v>81</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="13">
         <v>378</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E10" s="14">
         <v>374</v>
       </c>
-      <c r="F10" s="16">
+      <c r="F10" s="14">
         <v>374</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="18">
         <v>89</v>
       </c>
-      <c r="D11" s="16">
-        <v>392</v>
-      </c>
-      <c r="E11" s="16">
-        <v>382</v>
-      </c>
-      <c r="F11" s="15">
+      <c r="D11" s="14">
+        <v>396</v>
+      </c>
+      <c r="E11" s="14">
+        <v>395</v>
+      </c>
+      <c r="F11" s="13">
         <v>357</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="18">
         <v>96</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="13">
         <v>416</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="13">
         <v>397</v>
       </c>
-      <c r="F12" s="15">
+      <c r="F12" s="13">
         <v>354</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="18">
         <v>102</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="13">
         <v>412</v>
       </c>
-      <c r="E13" s="15">
-        <v>392</v>
-      </c>
-      <c r="F13" s="16">
+      <c r="E13" s="13">
+        <v>393</v>
+      </c>
+      <c r="F13" s="14">
         <v>386</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="18">
         <v>109</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="13">
         <v>435</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E14" s="13">
         <v>417</v>
       </c>
-      <c r="F14" s="15"/>
+      <c r="F14" s="13"/>
     </row>
     <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="18">
         <v>999</v>
       </c>
-      <c r="D15" s="16">
+      <c r="D15" s="14">
         <v>492</v>
       </c>
-      <c r="E15" s="15">
-        <v>432</v>
-      </c>
-      <c r="F15" s="4">
+      <c r="E15" s="13">
+        <v>436</v>
+      </c>
+      <c r="F15" s="18">
         <v>396</v>
       </c>
       <c r="H15" s="1" t="s">
@@ -879,230 +902,230 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="18">
         <v>35</v>
       </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="18">
         <v>40</v>
       </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="15">
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="13">
         <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="18">
         <v>45</v>
       </c>
-      <c r="D18" s="15">
+      <c r="D18" s="13">
         <v>191</v>
       </c>
-      <c r="E18" s="15">
+      <c r="E18" s="13">
         <v>179</v>
       </c>
-      <c r="F18" s="15">
+      <c r="F18" s="13">
         <v>172</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="18">
         <v>49</v>
       </c>
-      <c r="D19" s="16">
+      <c r="D19" s="14">
+        <v>216</v>
+      </c>
+      <c r="E19" s="13">
+        <v>206</v>
+      </c>
+      <c r="F19" s="13">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="18">
+        <v>55</v>
+      </c>
+      <c r="D20" s="13">
+        <v>233</v>
+      </c>
+      <c r="E20" s="14">
         <v>213</v>
       </c>
-      <c r="E19" s="15">
-        <v>206</v>
-      </c>
-      <c r="F19" s="15">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" s="1" t="s">
+      <c r="F20" s="14">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="4">
-        <v>55</v>
-      </c>
-      <c r="D20" s="15">
-        <v>227</v>
-      </c>
-      <c r="E20" s="16">
-        <v>212</v>
-      </c>
-      <c r="F20" s="16">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="18">
+        <v>59</v>
+      </c>
+      <c r="D21" s="14">
+        <v>247</v>
+      </c>
+      <c r="E21" s="13">
+        <v>246</v>
+      </c>
+      <c r="F21" s="13">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="4">
-        <v>59</v>
-      </c>
-      <c r="D21" s="16">
-        <v>247</v>
-      </c>
-      <c r="E21" s="15">
-        <v>228</v>
-      </c>
-      <c r="F21" s="15">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="18">
+        <v>64</v>
+      </c>
+      <c r="D22" s="13">
+        <v>261</v>
+      </c>
+      <c r="E22" s="13">
+        <v>240</v>
+      </c>
+      <c r="F22" s="13">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="4">
-        <v>64</v>
-      </c>
-      <c r="D22" s="15">
-        <v>261</v>
-      </c>
-      <c r="E22" s="15">
-        <v>240</v>
-      </c>
-      <c r="F22" s="15">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="18">
+        <v>71</v>
+      </c>
+      <c r="D23" s="13">
+        <v>273</v>
+      </c>
+      <c r="E23" s="13">
+        <v>253</v>
+      </c>
+      <c r="F23" s="14">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="4">
-        <v>71</v>
-      </c>
-      <c r="D23" s="15">
-        <v>267</v>
-      </c>
-      <c r="E23" s="15">
-        <v>252</v>
-      </c>
-      <c r="F23" s="16">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="1" t="s">
+      <c r="C24" s="18">
+        <v>76</v>
+      </c>
+      <c r="D24" s="13">
+        <v>278</v>
+      </c>
+      <c r="E24" s="13">
+        <v>259</v>
+      </c>
+      <c r="F24" s="13">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="4">
-        <v>76</v>
-      </c>
-      <c r="D24" s="15">
-        <v>278</v>
-      </c>
-      <c r="E24" s="15">
-        <v>259</v>
-      </c>
-      <c r="F24" s="15">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B25" s="1" t="s">
+      <c r="C25" s="18">
+        <v>81</v>
+      </c>
+      <c r="D25" s="13">
+        <v>283</v>
+      </c>
+      <c r="E25" s="13">
+        <v>260</v>
+      </c>
+      <c r="F25" s="13">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="4">
-        <v>81</v>
-      </c>
-      <c r="D25" s="15">
-        <v>283</v>
-      </c>
-      <c r="E25" s="15">
-        <v>260</v>
-      </c>
-      <c r="F25" s="15">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" s="1" t="s">
+      <c r="C26" s="18">
+        <v>87</v>
+      </c>
+      <c r="D26" s="13">
+        <v>294</v>
+      </c>
+      <c r="E26" s="13">
+        <v>269</v>
+      </c>
+      <c r="F26" s="13"/>
+    </row>
+    <row r="27" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="4">
-        <v>87</v>
-      </c>
-      <c r="D26" s="15">
-        <v>294</v>
-      </c>
-      <c r="E26" s="15">
-        <v>269</v>
-      </c>
-      <c r="F26" s="15"/>
-    </row>
-    <row r="27" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C27" s="4">
+      <c r="C27" s="18">
         <v>999</v>
       </c>
-      <c r="D27" s="16">
+      <c r="D27" s="14">
         <v>335</v>
       </c>
-      <c r="E27" s="15">
+      <c r="E27" s="13">
         <v>332</v>
       </c>
-      <c r="F27" s="4">
+      <c r="F27" s="18">
         <v>255</v>
       </c>
       <c r="H27" s="1" t="s">
@@ -1125,7 +1148,7 @@
   </sheetPr>
   <dimension ref="A1:U45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1152,11 +1175,11 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
       <c r="M1" s="6"/>

</xml_diff>